<commit_message>
Formatting fire stats table
</commit_message>
<xml_diff>
--- a/Tables/table1_firestats.xlsx
+++ b/Tables/table1_firestats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/New Mexico/USGS/Research/Swiss Cheese/Conchas_High_Severity/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EF0D120-D13B-A240-ABA2-BDDCE040F280}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1629F0BF-BA9B-D44E-A8E0-8DD09C067399}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6460" yWindow="2580" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
@@ -22,21 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>Fire</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Area_HS</t>
-  </si>
-  <si>
-    <t>Prop_HS</t>
-  </si>
-  <si>
     <t>Las Conchas</t>
   </si>
   <si>
@@ -56,13 +41,28 @@
   </si>
   <si>
     <t>Dome overlap</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>proportion high severity</t>
+  </si>
+  <si>
+    <t>high severity area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,6 +197,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -379,7 +385,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -494,6 +500,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -539,8 +554,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -898,134 +924,144 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+    <row r="1" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
         <v>2011</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>61057</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>21834</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>0.36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <v>2000</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>17919</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>6155</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0.34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
         <v>7799</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>2789</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
         <v>1998</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>2144</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>615</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
         <v>1952</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>605</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
         <v>1996</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>6385</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>1249</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
         <v>6320</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>1253</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>